<commit_message>
Add creation of new Household using HDS-Forms - Alpha Phase
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/hform_model.xlsx
+++ b/app/src/main/res/raw/hform_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11895" tabRatio="500"/>
+    <workbookView windowHeight="17295" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>group</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Codigo da Regiao</t>
   </si>
   <si>
-    <t>TXU</t>
-  </si>
-  <si>
     <t>region_name</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Nome da Regiao</t>
   </si>
   <si>
-    <t>Txumene</t>
-  </si>
-  <si>
     <t>household_code</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>Codigo do Agregado</t>
   </si>
   <si>
-    <t>TXUPF1005</t>
-  </si>
-  <si>
     <t>household_name</t>
   </si>
   <si>
@@ -100,9 +91,6 @@
   </si>
   <si>
     <t>Nome do Agregado</t>
-  </si>
-  <si>
-    <t>Just Me In</t>
   </si>
   <si>
     <t>Member Name</t>
@@ -281,10 +269,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -292,13 +280,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -309,6 +290,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -317,13 +305,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -335,20 +316,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -361,6 +328,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -369,46 +396,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,24 +426,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,79 +454,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,85 +622,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,11 +660,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,26 +707,20 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -748,148 +736,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1215,7 +1203,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1281,9 +1269,7 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
+      <c r="I2"/>
       <c r="J2" t="b">
         <v>1</v>
       </c>
@@ -1296,20 +1282,18 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
+      <c r="I3"/>
       <c r="J3" t="b">
         <v>1</v>
       </c>
@@ -1322,20 +1306,18 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I4"/>
       <c r="J4" t="b">
         <v>1</v>
       </c>
@@ -1345,20 +1327,18 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I5"/>
       <c r="J5" t="b">
         <v>1</v>
       </c>
@@ -1372,10 +1352,10 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -1384,19 +1364,19 @@
     <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1405,17 +1385,17 @@
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -1424,49 +1404,49 @@
     <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -1475,16 +1455,16 @@
     <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
@@ -1493,16 +1473,16 @@
     <row r="13" spans="1:11">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
@@ -1511,16 +1491,16 @@
     <row r="14" spans="1:11">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
@@ -1529,16 +1509,16 @@
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K15" t="b">
         <v>1</v>
@@ -1610,7 +1590,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1621,86 +1601,86 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1727,24 +1707,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add All Surveillance Forms to the app
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/hform_model.xlsx
+++ b/app/src/main/res/raw/hform_model.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17295" tabRatio="500"/>
+    <workbookView windowHeight="17670" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
     <sheet name="options" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
   <si>
     <t>group</t>
   </si>
@@ -36,6 +36,9 @@
     <t>options</t>
   </si>
   <si>
+    <t>foreach_count</t>
+  </si>
+  <si>
     <t>label</t>
   </si>
   <si>
@@ -45,10 +48,19 @@
     <t>default_value</t>
   </si>
   <si>
+    <t>calculation</t>
+  </si>
+  <si>
     <t>required</t>
   </si>
   <si>
     <t>readonly</t>
+  </si>
+  <si>
+    <t>display_condition</t>
+  </si>
+  <si>
+    <t>display_style</t>
   </si>
   <si>
     <t>header</t>
@@ -269,9 +281,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -291,9 +303,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,6 +324,104 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -313,13 +430,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -329,105 +439,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,13 +454,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,6 +514,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -472,43 +580,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,109 +622,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,8 +720,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,162 +740,162 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1005,7 +1017,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1026,9 +1038,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="true"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1049,7 +1061,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="false"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1119,7 +1131,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1145,7 +1157,7 @@
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1200,25 +1212,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="11.1428571428571" customWidth="true"/>
-    <col min="3" max="3" width="14.1428571428571" customWidth="true"/>
-    <col min="4" max="4" width="20.1428571428571" customWidth="true"/>
-    <col min="5" max="5" width="11.7142857142857" customWidth="true"/>
-    <col min="6" max="6" width="9.71428571428571" customWidth="true"/>
-    <col min="7" max="7" width="26.8571428571429" customWidth="true"/>
-    <col min="8" max="9" width="21.7142857142857" customWidth="true"/>
-    <col min="10" max="10" width="9.28571428571429" customWidth="true"/>
+    <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="9.71428571428571" customWidth="1"/>
+    <col min="7" max="7" width="13.7142857142857" customWidth="1"/>
+    <col min="8" max="8" width="26.8571428571429" customWidth="1"/>
+    <col min="9" max="11" width="21.7142857142857" customWidth="1"/>
+    <col min="12" max="12" width="9.28571428571429" customWidth="1"/>
+    <col min="14" max="14" width="16.5714285714286" customWidth="1"/>
+    <col min="15" max="15" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,275 +1267,286 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2"/>
-      <c r="J2" t="b">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="b">
         <v>1</v>
       </c>
-      <c r="K2" t="b">
+      <c r="M3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3" t="b">
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="b">
         <v>1</v>
       </c>
-      <c r="K3" t="b">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4"/>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="b">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="b">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" t="b">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1"/>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" t="b">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" t="b">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" t="b">
+        <v>58</v>
+      </c>
+      <c r="I13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" t="b">
+        <v>61</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" t="b">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1581,8 +1607,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="true"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="true"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1590,97 +1616,97 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1700,31 +1726,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="true"/>
-    <col min="2" max="2" width="20.4285714285714" customWidth="true"/>
-    <col min="3" max="3" width="23.2857142857143" customWidth="true"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="20.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="23.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>